<commit_message>
A long time I don't use Selenium
</commit_message>
<xml_diff>
--- a/AbbyCard/AbbyCard.xlsx
+++ b/AbbyCard/AbbyCard.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15270" windowHeight="6420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15270" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
     <sheet name="Login" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I18"/>
+  <oleSize ref="B1:H18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -135,26 +135,48 @@
     <t>TD10</t>
   </si>
   <si>
-    <t>thuyduong.trinhth1603+22@gmail.com</t>
-  </si>
-  <si>
-    <t>0166425900</t>
-  </si>
-  <si>
-    <t>TD22</t>
-  </si>
-  <si>
-    <t>Apache_POI_ TC 22</t>
-  </si>
-  <si>
-    <t>Thuy Duong test 22</t>
+    <t>TD23</t>
+  </si>
+  <si>
+    <t>0166425902</t>
+  </si>
+  <si>
+    <t>thuyduong.trinhth1603+23@gmail.com</t>
+  </si>
+  <si>
+    <t>Thuy Duong test 23</t>
+  </si>
+  <si>
+    <t>Apache_POI_ TC 23</t>
+  </si>
+  <si>
+    <t>Apache_POI_ TC 24</t>
+  </si>
+  <si>
+    <t>Thuy Duong test 24</t>
+  </si>
+  <si>
+    <t>TD24</t>
+  </si>
+  <si>
+    <t>0166425903</t>
+  </si>
+  <si>
+    <t>thuyduong.trinhth1603+24@gmail.com</t>
+  </si>
+  <si>
+    <t>123457</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,21 +564,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="42.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="23.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="42.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
+    <col min="9" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -587,19 +609,19 @@
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>11</v>
@@ -607,16 +629,32 @@
       <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -801,10 +839,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="thuyduong.trinhth1603@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="thuyduong.trinhth1603@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId5" display="thuyduong.trinhth1603@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -812,17 +851,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>